<commit_message>
Lower score for Tiny Toons 2
</commit_message>
<xml_diff>
--- a/My Sets/Tiny Toon Adventures 2 (Game Boy)/Tiny Toon Adventures 2 - Buster Bunny no Kattobi Daibouken - Plan.xlsx
+++ b/My Sets/Tiny Toon Adventures 2 (Game Boy)/Tiny Toon Adventures 2 - Buster Bunny no Kattobi Daibouken - Plan.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="126">
   <si>
     <t>Description</t>
   </si>
@@ -794,7 +794,7 @@
   <dimension ref="A1:G193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E33" sqref="E2:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,11 +844,11 @@
         <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E2" s="7">
         <f>VLOOKUP(D2,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>40</v>
@@ -866,11 +866,11 @@
         <v>81</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="7">
         <f>VLOOKUP(D3,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>41</v>
@@ -1404,11 +1404,11 @@
         <v>98</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" s="7">
         <f>VLOOKUP(D27,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>123</v>
@@ -1428,11 +1428,11 @@
         <v>100</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28" s="7">
         <f>VLOOKUP(D28,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>102</v>
@@ -3054,7 +3054,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3450,9 +3450,12 @@
       <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H12" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3480,9 +3483,12 @@
       <c r="G13" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H13" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3510,9 +3516,12 @@
       <c r="G14" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H14" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I14" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3540,9 +3549,12 @@
       <c r="G15" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H15" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3570,9 +3582,12 @@
       <c r="G16" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H16" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3864,9 +3879,12 @@
       <c r="G25" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H25" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I25" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3894,9 +3912,12 @@
       <c r="G26" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H26" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I26" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3924,9 +3945,12 @@
       <c r="G27" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H27" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I27" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3954,9 +3978,12 @@
       <c r="G28" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H28" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I28" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3984,9 +4011,12 @@
       <c r="G29" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H29" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I29" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4014,9 +4044,12 @@
       <c r="G30" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H30" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I30" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4044,9 +4077,12 @@
       <c r="G31" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H31" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I31" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4107,9 +4143,12 @@
       <c r="G33" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H33" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I33" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4133,11 +4172,11 @@
       </c>
       <c r="H34" s="7" t="str">
         <f>COUNTIF(H2:H33,"X")&amp;" /"&amp;ROW()-2</f>
-        <v>19 /32</v>
+        <v>32 /32</v>
       </c>
       <c r="I34" s="7" t="str">
         <f>COUNTIF(I2:I33,"YES")&amp;" /"&amp;ROW()-2</f>
-        <v>19 /32</v>
+        <v>32 /32</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4193,13 +4232,13 @@
     <row r="3" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="str">
         <f ca="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("Hop-along Little Buster","Beat the western movie", 2, trigger)</v>
+        <v>achievement("Hop-along Little Buster","Beat the western movie", 5, trigger)</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
         <f t="shared" ref="A4:A32" ca="1" si="0">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("The Twilight Samurai","Beat the samurai movie", 3, trigger)</v>
+        <v>achievement("The Twilight Samurai","Beat the samurai movie", 5, trigger)</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4343,13 +4382,13 @@
     <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Buster the Rocket","Beat the future movie with 260s or more left in the clock", 25, trigger)</v>
+        <v>achievement("Buster the Rocket","Beat the future movie with 260s or more left in the clock", 10, trigger)</v>
       </c>
     </row>
     <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Buster the Were-Rabbit","Beat the monster movie with 300s or more left in the clock", 25, trigger)</v>
+        <v>achievement("Buster the Were-Rabbit","Beat the monster movie with 300s or more left in the clock", 10, trigger)</v>
       </c>
     </row>
     <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4696,7 +4735,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUMIF(Achievements!B:B,E2,Achievements!E:E)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -4733,7 +4772,7 @@
       </c>
       <c r="C4">
         <f>COUNTIF(Achievements!D:D,A4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>34</v>
@@ -4744,7 +4783,7 @@
       </c>
       <c r="G4" s="7">
         <f>SUMIF(Achievements!B:B,E4,Achievements!E:E)</f>
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4756,7 +4795,7 @@
       </c>
       <c r="C5">
         <f>COUNTIF(Achievements!D:D,A5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>37</v>
@@ -4802,7 +4841,7 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Achievements!D:D,A7)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>5</v>
@@ -4813,7 +4852,7 @@
       </c>
       <c r="G7" s="3">
         <f>SUM(G2:G6)</f>
-        <v>295</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -4825,7 +4864,7 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Achievements!D:D,A8)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -4837,7 +4876,7 @@
       </c>
       <c r="C9" s="7">
         <f>COUNTIF(Achievements!D:D,A9)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>